<commit_message>
Getting started on validating the csv
</commit_message>
<xml_diff>
--- a/ASHRAE 229_maps_from_meeting_11.20.xlsx
+++ b/ASHRAE 229_maps_from_meeting_11.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AntonSzilasi\Documents\OpenStudio%20RPD%20Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2DA1249-D5E5-480A-852C-6DDB0ADA4409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116A5708-94DE-4F9C-BCCD-336E8CC521E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2656F7D-5FB8-4109-9F4A-1294C4A0C904}"/>
   </bookViews>
@@ -1038,7 +1038,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1078,12 +1078,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1513,8 +1507,8 @@
   <dimension ref="A1:F257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2668,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>110</v>
       </c>
@@ -2686,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>110</v>
       </c>
@@ -6177,6 +6171,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="141d59ff-0f67-4f50-8344-64b15536f9a6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b95255b-60dc-4683-a12c-6b4df4508597">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002623BFAE8B0C414481CE00A23BDDDF22" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5757300bcb8c7282e444b5e121d16c6e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="141d59ff-0f67-4f50-8344-64b15536f9a6" xmlns:ns3="2b95255b-60dc-4683-a12c-6b4df4508597" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dd4915a0a1810b23a552d1776a3d509" ns2:_="" ns3:_="">
     <xsd:import namespace="141d59ff-0f67-4f50-8344-64b15536f9a6"/>
@@ -6431,17 +6436,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="141d59ff-0f67-4f50-8344-64b15536f9a6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b95255b-60dc-4683-a12c-6b4df4508597">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{990887CD-D250-4ED0-A47A-4E0527CF5605}">
   <ds:schemaRefs>
@@ -6451,6 +6445,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD55297-B292-4293-97C1-FE88096D455C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="141d59ff-0f67-4f50-8344-64b15536f9a6"/>
+    <ds:schemaRef ds:uri="2b95255b-60dc-4683-a12c-6b4df4508597"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BE155D2-63C4-4303-8EFD-5DA9AEB30886}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6467,15 +6472,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD55297-B292-4293-97C1-FE88096D455C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="141d59ff-0f67-4f50-8344-64b15536f9a6"/>
-    <ds:schemaRef ds:uri="2b95255b-60dc-4683-a12c-6b4df4508597"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>